<commit_message>
Comments updated in excel sheet
</commit_message>
<xml_diff>
--- a/Water/Flow based smart irrigation/flow_based_smart_irrigation_master.xlsx
+++ b/Water/Flow based smart irrigation/flow_based_smart_irrigation_master.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="42">
   <si>
     <t>Objective</t>
   </si>
@@ -139,6 +139,9 @@
   </si>
   <si>
     <t>Working video</t>
+  </si>
+  <si>
+    <t>What to modify in code? -  What parameter is on what line in the code as what variable?</t>
   </si>
 </sst>
 </file>
@@ -162,7 +165,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -172,6 +175,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -188,7 +197,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -197,6 +206,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -257,7 +267,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -292,7 +302,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -507,9 +517,9 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.7109375" customWidth="1"/>
+    <col min="1" max="1" width="27.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -579,11 +589,11 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -661,18 +671,18 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="42.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="50.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="50.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.44140625" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>23</v>
       </c>
@@ -684,7 +694,7 @@
       </c>
       <c r="D1" s="4"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -695,7 +705,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -706,23 +716,23 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="C6" s="3" t="s">
         <v>30</v>
       </c>
       <c r="D6" s="6"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>3</v>
       </c>
@@ -733,22 +743,22 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>4</v>
       </c>
@@ -759,22 +769,22 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>5</v>
       </c>
@@ -782,15 +792,19 @@
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>6</v>
       </c>
       <c r="B16" t="s">
         <v>11</v>
       </c>
+      <c r="C16" s="8" t="s">
+        <v>41</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>